<commit_message>
balanced latin square cleanup
</commit_message>
<xml_diff>
--- a/experiment/BalancedLatinSquare.xlsx
+++ b/experiment/BalancedLatinSquare.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="64">
   <si>
     <t>IV 2: Weight</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>OW_F_UCB</t>
+  </si>
+  <si>
+    <t>Subject #</t>
   </si>
 </sst>
 </file>
@@ -264,7 +267,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -324,6 +327,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -332,7 +346,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -366,6 +380,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -650,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="V31" sqref="V31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1254,6 +1271,9 @@
       <c r="H27" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="I27" s="12" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
@@ -1273,6 +1293,9 @@
       <c r="H28" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
@@ -1292,6 +1315,9 @@
       <c r="H29" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="I29">
+        <v>2</v>
+      </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
@@ -1311,6 +1337,9 @@
       <c r="H30" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="I30">
+        <v>3</v>
+      </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
@@ -1330,6 +1359,9 @@
       <c r="H31" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="I31">
+        <v>4</v>
+      </c>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
@@ -1349,8 +1381,11 @@
       <c r="H32" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
         <v>33</v>
       </c>
@@ -1368,8 +1403,11 @@
       <c r="H33" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
         <v>34</v>
       </c>
@@ -1387,8 +1425,11 @@
       <c r="H34" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
         <v>35</v>
       </c>
@@ -1406,8 +1447,11 @@
       <c r="H35" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
         <v>36</v>
       </c>
@@ -1425,8 +1469,11 @@
       <c r="H36" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I36">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
         <v>37</v>
       </c>
@@ -1444,8 +1491,11 @@
       <c r="H37" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
         <v>38</v>
       </c>
@@ -1463,8 +1513,11 @@
       <c r="H38" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I38">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
         <v>39</v>
       </c>
@@ -1482,8 +1535,11 @@
       <c r="H39" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I39">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B40" s="6" t="s">
         <v>40</v>
       </c>
@@ -1501,8 +1557,11 @@
       <c r="H40" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I40">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
         <v>41</v>
       </c>
@@ -1520,8 +1579,11 @@
       <c r="H41" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I41">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
         <v>42</v>
       </c>
@@ -1539,8 +1601,11 @@
       <c r="H42" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I42">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
         <v>43</v>
       </c>
@@ -1557,6 +1622,9 @@
       </c>
       <c r="H43" s="2" t="s">
         <v>60</v>
+      </c>
+      <c r="I43">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1621,5 +1689,6 @@
     <mergeCell ref="J22:L22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated stimuli names and balanced latin square table
</commit_message>
<xml_diff>
--- a/experiment/BalancedLatinSquare.xlsx
+++ b/experiment/BalancedLatinSquare.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
-  <workbookPr/>
+  <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shawn/Developer/psych100b_exp/Psych100B-Experiment/experiment/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="68">
   <si>
     <t>IV 2: Weight</t>
   </si>
@@ -219,13 +219,25 @@
   </si>
   <si>
     <t>Subject #</t>
+  </si>
+  <si>
+    <t>John Curtis</t>
+  </si>
+  <si>
+    <t>Jane Conner</t>
+  </si>
+  <si>
+    <t>Jake Cooper</t>
+  </si>
+  <si>
+    <t>Jill Carter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -258,13 +270,81 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -329,24 +409,33 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -363,33 +452,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="8" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="8" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="8" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="9" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="9" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="10">
+    <cellStyle name="Bad" xfId="6" builtinId="27"/>
+    <cellStyle name="Calculation" xfId="9" builtinId="22"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="5" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Input" xfId="8" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="7" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -668,144 +804,161 @@
   <dimension ref="B1:P43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="V31" sqref="V31"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="12" max="12" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
       <c r="H4" s="9"/>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="9"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="9"/>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>2</v>
       </c>
       <c r="H5" s="9"/>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="26" t="s">
         <v>6</v>
       </c>
+      <c r="L5" s="26" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6" t="s">
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="J6" s="2" t="s">
+      <c r="H6" s="10"/>
+      <c r="J6" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="26" t="s">
         <v>8</v>
       </c>
+      <c r="L6" s="26" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B7" s="7"/>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6" t="s">
+      <c r="D7" s="10"/>
+      <c r="E7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6" t="s">
+      <c r="F7" s="10"/>
+      <c r="G7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="J7" s="2" t="s">
+      <c r="H7" s="10"/>
+      <c r="J7" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="26" t="s">
         <v>7</v>
       </c>
+      <c r="L7" s="26" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="26" t="s">
         <v>9</v>
       </c>
+      <c r="L8" s="26" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6" t="s">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
       <c r="I10" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6" t="s">
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
       <c r="E11" s="1" t="s">
         <v>26</v>
       </c>
@@ -821,11 +974,11 @@
       <c r="I11" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
       <c r="M11" s="1" t="s">
         <v>26</v>
       </c>
@@ -840,11 +993,11 @@
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B12" s="6">
+      <c r="B12" s="10">
         <v>1</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
@@ -860,11 +1013,11 @@
       <c r="I12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="10">
         <v>1</v>
       </c>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
       <c r="M12" s="2" t="s">
         <v>6</v>
       </c>
@@ -879,11 +1032,11 @@
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B13" s="6">
+      <c r="B13" s="10">
         <v>2</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
       <c r="E13" s="2" t="s">
         <v>15</v>
       </c>
@@ -899,11 +1052,11 @@
       <c r="I13" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="10">
         <v>2</v>
       </c>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
       <c r="M13" s="2" t="s">
         <v>8</v>
       </c>
@@ -918,11 +1071,11 @@
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B14" s="6">
+      <c r="B14" s="10">
         <v>3</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
       <c r="E14" s="2" t="s">
         <v>16</v>
       </c>
@@ -938,11 +1091,11 @@
       <c r="I14" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J14" s="10">
         <v>3</v>
       </c>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
       <c r="M14" s="2" t="s">
         <v>7</v>
       </c>
@@ -957,11 +1110,11 @@
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B15" s="6">
+      <c r="B15" s="10">
         <v>4</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
       <c r="E15" s="2" t="s">
         <v>17</v>
       </c>
@@ -977,11 +1130,11 @@
       <c r="I15" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15" s="10">
         <v>4</v>
       </c>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
       <c r="M15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1016,34 +1169,34 @@
       <c r="I17" s="5"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6" t="s">
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
       <c r="I18" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6" t="s">
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
       <c r="E19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1059,11 +1212,11 @@
       <c r="I19" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J19" s="6" t="s">
+      <c r="J19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
       <c r="M19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1078,11 +1231,11 @@
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B20" s="6">
+      <c r="B20" s="10">
         <v>1</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
       <c r="E20" s="2" t="s">
         <v>14</v>
       </c>
@@ -1098,11 +1251,11 @@
       <c r="I20" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J20" s="10">
         <v>1</v>
       </c>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
       <c r="M20" s="2" t="s">
         <v>6</v>
       </c>
@@ -1117,11 +1270,11 @@
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B21" s="6">
+      <c r="B21" s="10">
         <v>2</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
       <c r="E21" s="2" t="s">
         <v>15</v>
       </c>
@@ -1137,11 +1290,11 @@
       <c r="I21" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J21" s="6">
+      <c r="J21" s="10">
         <v>2</v>
       </c>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
       <c r="M21" s="2" t="s">
         <v>8</v>
       </c>
@@ -1156,11 +1309,11 @@
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B22" s="6">
+      <c r="B22" s="10">
         <v>3</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
       <c r="E22" s="2" t="s">
         <v>16</v>
       </c>
@@ -1176,11 +1329,11 @@
       <c r="I22" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J22" s="6">
+      <c r="J22" s="10">
         <v>3</v>
       </c>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
       <c r="M22" s="2" t="s">
         <v>7</v>
       </c>
@@ -1195,11 +1348,11 @@
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B23" s="6">
+      <c r="B23" s="10">
         <v>4</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -1215,11 +1368,11 @@
       <c r="I23" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J23" s="6">
+      <c r="J23" s="10">
         <v>4</v>
       </c>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
       <c r="M23" s="2" t="s">
         <v>9</v>
       </c>
@@ -1243,22 +1396,23 @@
       <c r="H24" s="3"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="6" t="s">
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
       <c r="E27" s="4" t="s">
         <v>22</v>
       </c>
@@ -1276,375 +1430,389 @@
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="2" t="s">
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H28" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="2" t="s">
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="H29" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="2" t="s">
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H30" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="21">
         <v>3</v>
       </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="2" t="s">
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H31" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="21">
         <v>4</v>
       </c>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="2" t="s">
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G32" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="H32" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="22">
         <v>5</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="2" t="s">
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="H33" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="22">
         <v>6</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="2" t="s">
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="H34" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="22">
         <v>7</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="2" t="s">
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G35" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="H35" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="I35">
+      <c r="I35" s="22">
         <v>8</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="2" t="s">
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="H36" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="23">
         <v>9</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="2" t="s">
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G37" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="H37" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="I37">
+      <c r="I37" s="23">
         <v>10</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="2" t="s">
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G38" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="H38" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="I38">
+      <c r="I38" s="23">
         <v>11</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="2" t="s">
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="G39" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="H39" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="23">
         <v>12</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="2" t="s">
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="G40" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H40" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="I40">
+      <c r="I40" s="24">
         <v>13</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="2" t="s">
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F41" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G41" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="H41" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="24">
         <v>14</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="2" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F42" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G42" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="H42" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="24">
         <v>15</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="2" t="s">
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F43" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="G43" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="H43" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="I43">
+      <c r="I43" s="24">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="B1:H2"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="M18:P18"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="M10:P10"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
     <mergeCell ref="E18:H18"/>
-    <mergeCell ref="J4:K4"/>
     <mergeCell ref="B26:D27"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="B29:D29"/>
@@ -1659,34 +1827,20 @@
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E26:H26"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="M10:P10"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="M18:P18"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B1:H2"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>